<commit_message>
Add BaseVariate AryAry Type
</commit_message>
<xml_diff>
--- a/Assets/Config/Excel/Test.xlsx
+++ b/Assets/Config/Excel/Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitPorject\ScriptImoprt\Assets\Config\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF5D505-66FD-48A4-BA62-EA2645E604EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8819AD3-F292-4DE5-8F29-B40D727523E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6630" yWindow="3360" windowWidth="26115" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -416,7 +416,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>